<commit_message>
new sentences to annotate
</commit_message>
<xml_diff>
--- a/ENg_ANN_golddata.xlsx
+++ b/ENg_ANN_golddata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ituniversity-my.sharepoint.com/personal/jhag_itu_dk/Documents/NLP/NLP_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{9F75503D-D61A-E242-9F27-57233EC2EFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04833CF3-1CF6-AF42-978A-2D39DF0EA738}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{9F75503D-D61A-E242-9F27-57233EC2EFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB70E814-3600-2242-B3E5-A46B4F82554A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{6CD1853F-A450-BF4F-90EC-653684AB6D3F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{6CD1853F-A450-BF4F-90EC-653684AB6D3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="477">
   <si>
     <t>[]</t>
   </si>
@@ -609,13 +609,871 @@
   </si>
   <si>
     <t xml:space="preserve">[0,0,0,0,0,0,0,3] </t>
+  </si>
+  <si>
+    <t>[ "''", "Autosticha", "pelodes", "''", "Meyrick", ",", "1928" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 5, 6, 0, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "en", "en", "en", "en", "en", "en", "en" ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Autosticha pelodes" ]</t>
+  </si>
+  <si>
+    <t>[ "Cities", "Built", "on", "Sand" ]</t>
+  </si>
+  <si>
+    <t>[ 5, 6, 6, 6 ]</t>
+  </si>
+  <si>
+    <t>[ "en", "en", "en", "en" ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Cities Built on Sand" ]</t>
+  </si>
+  <si>
+    <t>[ "It", "was", "originally", "recorded", "by", "The", "Great", "Society", ",", "and", "later", "by", "Jefferson", "Airplane", "." ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 0, 0, 0, 3, 4, 4, 0, 0, 0, 0, 3, 4, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en" ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: The Great Society", "ORG: Jefferson Airplane" ]</t>
+  </si>
+  <si>
+    <t>[ "H.", "T.", "Bartlett", "1947–1949" ]</t>
+  </si>
+  <si>
+    <t>[ 1, 2, 2, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "PER: H. T. Bartlett" ]</t>
+  </si>
+  <si>
+    <t>[ "'", "''", "Mittani", "''", "'" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 3, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "en", "en", "en", "en", "en" ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Mittani" ]</t>
+  </si>
+  <si>
+    <t>[ "Its", "local", "government", "area", "are", "the", "Cities", "of", "Boroondara", "and", "Stonnington", "." ]</t>
+  </si>
+  <si>
+    <t>[ 0, 3, 4, 4, 0, 0, 0, 0, 5, 0, 5, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en" ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: local government area", "LOC: Boroondara", "LOC: Stonnington" ]</t>
+  </si>
+  <si>
+    <t>[ "Martín", "de", "Ursúa" ]</t>
+  </si>
+  <si>
+    <t>[ 1, 2, 2 ]</t>
+  </si>
+  <si>
+    <t>[ "en", "en", "en" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Martín de Ursúa" ]</t>
+  </si>
+  <si>
+    <t>[ "Zawadzkie", ",", "Kolonowskie", ",", "Leśnica", ",", "Ujazd" ]</t>
+  </si>
+  <si>
+    <t>[ 5, 0, 5, 0, 5, 0, 5 ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Zawadzkie", "LOC: Kolonowskie", "LOC: Leśnica", "LOC: Ujazd" ]</t>
+  </si>
+  <si>
+    <t>[ "Orange", ",", "New", "South", "Wales" ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Orange , New South Wales" ]</t>
+  </si>
+  <si>
+    <t>[ "Göttingen", "State", "and", "University", "Library", ",", "Göttingen" ]</t>
+  </si>
+  <si>
+    <t>[ 3, 4, 4, 4, 4, 0, 5 ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Göttingen State and University Library", "LOC: Göttingen" ]</t>
+  </si>
+  <si>
+    <t>[ "'", "''", "Uganda", "''", "'" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 5, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Uganda" ]</t>
+  </si>
+  <si>
+    <t>[ "Dwarf", "flying", "fox" ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Dwarf flying fox" ]</t>
+  </si>
+  <si>
+    <t>[ "In", "1989", ",", "he", "joined", "Rapho", "agency", "and", "spent", "one", "year", "in", "Egypt", "." ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 0, 0, 0, 3, 4, 0, 0, 0, 0, 0, 5, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en" ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Rapho agency", "LOC: Egypt" ]</t>
+  </si>
+  <si>
+    <t>[ "Ruth", "Bryan", "Owen", "was", "also", "a", "granddaughter", "." ]</t>
+  </si>
+  <si>
+    <t>[ 1, 2, 2, 0, 0, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "en", "en", "en", "en", "en", "en", "en", "en" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Ruth Bryan Owen" ]</t>
+  </si>
+  <si>
+    <t>[ "Skegness", "Town", "A.F.C", "." ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Skegness Town A.F.C ." ]</t>
+  </si>
+  <si>
+    <t>[ "Horisme", "aquata", "''", "(", "Hübner", ",", "1813", ")" ]</t>
+  </si>
+  <si>
+    <t>[ 5, 6, 0, 0, 0, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Horisme aquata" ]</t>
+  </si>
+  <si>
+    <t>[ "The", "Young", "Indiana", "Jones", "Chronicles", "''" ]</t>
+  </si>
+  <si>
+    <t>[ 1, 2, 2, 2, 2, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "en", "en", "en", "en", "en", "en" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: The Young Indiana Jones Chronicles" ]</t>
+  </si>
+  <si>
+    <t>[ "Matthias", "Bachinger", "Ričardas", "Berankis", "Niels", "Desein", "Pere", "Riba" ]</t>
+  </si>
+  <si>
+    <t>[ 1, 2, 1, 2, 1, 2, 1, 2 ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Matthias Bachinger", "PER: Ričardas Berankis", "PER: Niels Desein", "PER: Pere Riba" ]</t>
+  </si>
+  <si>
+    <t>[ "Little", "River", "(", "Cariboo", "River", ")" ]</t>
+  </si>
+  <si>
+    <t>[ 5, 6, 6, 6, 6, 6 ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Little River ( Cariboo River )" ]</t>
+  </si>
+  <si>
+    <t>[ "Grangettes", ",", "Marsens", ",", "Sâles", ",", "Riaz" ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Grangettes", "LOC: Marsens", "LOC: Sâles", "LOC: Riaz" ]</t>
+  </si>
+  <si>
+    <t>[ "The", "Little", "Mermaid", "2", ":", "Return", "to", "the", "Sea", "''" ]</t>
+  </si>
+  <si>
+    <t>[ 3, 4, 4, 4, 4, 4, 4, 4, 4, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "en", "en", "en", "en", "en", "en", "en", "en", "en", "en" ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: The Little Mermaid 2 : Return to the Sea" ]</t>
+  </si>
+  <si>
+    <t>[ ":", "Ross", "Dowson", "-", "4,539" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 1, 2, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Ross Dowson" ]</t>
+  </si>
+  <si>
+    <t>[ "``", "Dead", "on", "Arrival", "''", "-", "Fall", "Out", "Boy" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 3, 4, 4, 0, 0, 3, 4, 4 ]</t>
+  </si>
+  <si>
+    <t>[ "en", "en", "en", "en", "en", "en", "en", "en", "en" ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Dead on Arrival", "ORG: Fall Out Boy" ]</t>
+  </si>
+  <si>
+    <t>[ "Lists", "of", "violinists" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Lists of violinists" ]</t>
+  </si>
+  <si>
+    <t>[ "SPÖ", "(", "'Labour", "'", ")" ]</t>
+  </si>
+  <si>
+    <t>[ 3, 0, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: SPÖ" ]</t>
+  </si>
+  <si>
+    <t>[ "'", "''", "Trisha", "Chetty", "''", "'" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 1, 2, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Trisha Chetty" ]</t>
+  </si>
+  <si>
+    <t>[ "Harry", "Gordon", "(", "disambiguation", ")" ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Harry Gordon ( disambiguation )" ]</t>
+  </si>
+  <si>
+    <t>[ "Axtell", "High", "School", "(", "disambiguation", ")" ]</t>
+  </si>
+  <si>
+    <t>[ 3, 4, 4, 4, 4, 4 ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Axtell High School ( disambiguation )" ]</t>
+  </si>
+  <si>
+    <t>[ "St.", "Louis", "Wrestling", "Hall", "of", "Fame" ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: St. Louis Wrestling Hall of Fame" ]</t>
+  </si>
+  <si>
+    <t>[ "Cultural", "heritage", "sites", "in", "FATA" ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Cultural heritage sites in FATA" ]</t>
+  </si>
+  <si>
+    <t>[ "William", "Joseph", "McInnes", "Botanic", "Garden", "and", "Campus", "Arboretum" ]</t>
+  </si>
+  <si>
+    <t>[ 5, 6, 6, 6, 6, 6, 6, 6 ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: William Joseph McInnes Botanic Garden and Campus Arboretum" ]</t>
+  </si>
+  <si>
+    <t>[ "1st", "King", "'s", "Dragoon", "Guards", "''", "(", "from", "26", "February", "until", "22", "March", "1941", ")", "''" ]</t>
+  </si>
+  <si>
+    <t>[ 3, 4, 4, 4, 4, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en" ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: 1st King 's Dragoon Guards" ]</t>
+  </si>
+  <si>
+    <t>[ "**", "Wang", "Zhaozuo", "(", "王昭祚", ")", "(", "killed", "by", "Zhang", "Wenli", "921", ")" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 1, 2, 0, 0, 0, 0, 0, 0, 1, 2, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Wang Zhaozuo", "PER: Zhang Wenli" ]</t>
+  </si>
+  <si>
+    <t>[ "George", ",", "Duke", "of", "Saxony", ",", "1471", "–", "1539" ]</t>
+  </si>
+  <si>
+    <t>[ 1, 2, 2, 2, 2, 0, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "PER: George , Duke of Saxony" ]</t>
+  </si>
+  <si>
+    <t>[ "Borough", "of", "Bedford" ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Borough of Bedford" ]</t>
+  </si>
+  <si>
+    <t>[ "Feliks", "Kazimierz", "Potocki", "(", "1682", ")" ]</t>
+  </si>
+  <si>
+    <t>[ 1, 2, 2, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Feliks Kazimierz Potocki" ]</t>
+  </si>
+  <si>
+    <t>[ "Imre", "Nagy", "(", "1896–1958", ")" ]</t>
+  </si>
+  <si>
+    <t>[ 1, 2, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Imre Nagy" ]</t>
+  </si>
+  <si>
+    <t>[ "Trawlers", "of", "the", "Royal", "Navy" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Trawlers of the Royal Navy" ]</t>
+  </si>
+  <si>
+    <t>[ "James", "Scullin", "(", "22", "October", "1929", "–", "6", "January", "1932", ")" ]</t>
+  </si>
+  <si>
+    <t>[ 1, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: James Scullin" ]</t>
+  </si>
+  <si>
+    <t>[ "Macaria", "granitata", "''", "–", "Guenée", ",", "1857", "-", "Granite", "Moth" ]</t>
+  </si>
+  <si>
+    <t>[ 5, 6, 0, 0, 1, 0, 0, 0, 3, 4 ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Macaria granitata", "PER: Guenée", "ORG: Granite Moth" ]</t>
+  </si>
+  <si>
+    <t>[ "''", "Pyrausta", "virginalis", "''", "Duponchel", ",", "1832" ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Pyrausta virginalis" ]</t>
+  </si>
+  <si>
+    <t>[ "Colebrookdale", "Township", ",", "Berks", "County", ",", "Pennsylvania" ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Colebrookdale Township , Berks County , Pennsylvania" ]</t>
+  </si>
+  <si>
+    <t>[ "Matthew", "Farhang", "Mohtadi" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Matthew Farhang Mohtadi" ]</t>
+  </si>
+  <si>
+    <t>[ "911th", "Air", "Refueling", "Squadron", ":", "30", "September", "1982", "–", "22", "April", "1991" ]</t>
+  </si>
+  <si>
+    <t>[ 3, 4, 4, 4, 0, 0, 0, 0, 0, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: 911th Air Refueling Squadron" ]</t>
+  </si>
+  <si>
+    <t>[ "Communes", "of", "the", "Territoire", "de", "Belfort", "department" ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Communes of the Territoire de Belfort department" ]</t>
+  </si>
+  <si>
+    <t>[ "Francisco", "Espoz", "y", "Mina" ]</t>
+  </si>
+  <si>
+    <t>[ 1, 2, 2, 2 ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Francisco Espoz y Mina" ]</t>
+  </si>
+  <si>
+    <t>[ "'", "''", "Crazy", "Love", "Tour", "''", "'" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 3, 4, 4, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Crazy Love Tour" ]</t>
+  </si>
+  <si>
+    <t>[ ":", "Chief", "Justice", "of", "Nepal" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 3, 4, 4, 4 ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Chief Justice of Nepal" ]</t>
+  </si>
+  <si>
+    <t>[ ":", "Big", "FM", "(", "7.74", "%", ")" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 3, 4, 0, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Big FM" ]</t>
+  </si>
+  <si>
+    <t>[ "It", "is", "from", "the", "Pathanamthitta", "district", "headquarters", "." ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 0, 0, 5, 6, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Pathanamthitta district" ]</t>
+  </si>
+  <si>
+    <t>[ "13", "Kevin", "Riley", "-", "''Freshman", "''" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 3, 4, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Kevin Riley" ]</t>
+  </si>
+  <si>
+    <t>[ "Its", "headquarters", "are", "in", "Guatemala", "City", "." ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 0, 0, 5, 6, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Guatemala City" ]</t>
+  </si>
+  <si>
+    <t>[ "Rumba]]", "/", "``", "Waiting", "on", "the", "World", "to", "Change", "''" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 0, 3, 4, 4, 4, 4, 4, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Waiting on the World to Change" ]</t>
+  </si>
+  <si>
+    <t>[ "She", "later", "slept", "with", "Charlotte", "Lau", "(", "Amy", "Yamazaki", ")", "." ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 0, 0, 1, 2, 0, 1, 2, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Charlotte Lau", "PER: Amy Yamazaki" ]</t>
+  </si>
+  <si>
+    <t>[ "Armani", "Jeans", "Milano", "68–72", "Khimki", "Moscow", "Region" ]</t>
+  </si>
+  <si>
+    <t>[ 3, 4, 4, 0, 3, 4, 4 ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Armani Jeans Milano", "ORG: Khimki Moscow Region" ]</t>
+  </si>
+  <si>
+    <t>[ "(", "with", "Daniel", "Ryan", ")" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 1, 2, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Daniel Ryan" ]</t>
+  </si>
+  <si>
+    <t>[ "Sara", "C.", "Bisel" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Sara C. Bisel" ]</t>
+  </si>
+  <si>
+    <t>[ "She", "was", "launched", "in", "1936", "and", "was", "sunk", "during", "the", "Second", "World", "War", "." ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 3, 4, 4, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Second World War" ]</t>
+  </si>
+  <si>
+    <t>[ "William", "B.", "Buffum" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: William B. Buffum" ]</t>
+  </si>
+  <si>
+    <t>[ "''", "Daddy", "at", "Home", "''", "企鹅爸爸" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 3, 4, 4, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Daddy at Home" ]</t>
+  </si>
+  <si>
+    <t>[ "He", "was", "a", "member", "of", "the", "Maine", "House", "of", "Representatives", "in", "1862", ",", "1864", ",", "1866", "and", "1872", "and", "was", "a", "delegate", "to", "the", "Republican", "National", "Convention", "in", "1864", "." ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 0, 0, 0, 0, 3, 4, 4, 4, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 3, 4, 4, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en" ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Maine House of Representatives", "ORG: Republican National Convention" ]</t>
+  </si>
+  <si>
+    <t>[ "20px", "'", "''", "Starachowice", "''", "'" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 0, 5, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Starachowice" ]</t>
+  </si>
+  <si>
+    <t>[ "Szema", "Wah", "Lung", "as", "Baijun" ]</t>
+  </si>
+  <si>
+    <t>[ 1, 2, 2, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Szema Wah Lung" ]</t>
+  </si>
+  <si>
+    <t>[ ":", "Paul", "Nicholson", "''", "(", "Third", "round", ")" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 1, 2, 0, 0, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Paul Nicholson" ]</t>
+  </si>
+  <si>
+    <t>[ "``", "I", "Want", "More", "''", "(", "Can", "song", ")", ",", "a", "1976", "song", "by", "Can" ]</t>
+  </si>
+  <si>
+    <t>[ 3, 4, 4, 4, 4, 4, 4, 4, 4, 0, 0, 0, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: `` I Want More '' ( Can song )" ]</t>
+  </si>
+  <si>
+    <t>[ "It", "originated", "in", "Jamaica", ",", "North", "America", "and", "Europe", ",", "and", "first", "became", "popular", "in", "the", "late", "1990s", "." ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 0, 5, 0, 5, 6, 0, 5, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en" ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Jamaica", "LOC: North America", "LOC: Europe" ]</t>
+  </si>
+  <si>
+    <t>[ "KKCEM", "Dhanbad", "was", "established", "in", "the", "year", "of", "2011", "." ]</t>
+  </si>
+  <si>
+    <t>[ 0, 5, 0, 0, 0, 0, 0, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Dhanbad" ]</t>
+  </si>
+  <si>
+    <t>[ "The", "survivors", "were", "put", "ashore", "at", "Karlskrona", ",", "Sweden", "." ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 0, 0, 0, 0, 5, 0, 5, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Karlskrona", "LOC: Sweden" ]</t>
+  </si>
+  <si>
+    <t>[ "J.", "H.", "Hobart", "Ward" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: J. H. Hobart Ward" ]</t>
+  </si>
+  <si>
+    <t>[ "Thomas", "Langdon", "Grace" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Thomas Langdon Grace" ]</t>
+  </si>
+  <si>
+    <t>[ "Stephen", "Levin", "(", "councillor", ")" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Stephen Levin ( councillor )" ]</t>
+  </si>
+  <si>
+    <t>[ "Ilinka", "Mitreva", "(", "2002-2006", ")" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Ilinka Mitreva" ]</t>
+  </si>
+  <si>
+    <t>[ "Charlie", "Brown", "tries", "to", "sell", "wreaths", "door-to-door", "." ]</t>
+  </si>
+  <si>
+    <t>[ 1, 2, 0, 0, 0, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Charlie Brown" ]</t>
+  </si>
+  <si>
+    <t>[ "Przerębska", "Huta", ",", "Kościerzyna", "County" ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Przerębska Huta , Kościerzyna County" ]</t>
+  </si>
+  <si>
+    <t>[ "New", "York", "2,372,949", "(", "12.1", "%", ")" ]</t>
+  </si>
+  <si>
+    <t>[ 5, 6, 0, 0, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: New York" ]</t>
+  </si>
+  <si>
+    <t>[ "'", "''", "Elton", "John", "''", "'", "and", "'", "''", "Kiki", "Dee", "''", "'" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 1, 2, 0, 0, 0, 0, 0, 1, 2, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Elton John", "PER: Kiki Dee" ]</t>
+  </si>
+  <si>
+    <t>[ "Stephen", "Kosgei", "Kibet" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Stephen Kosgei Kibet" ]</t>
+  </si>
+  <si>
+    <t>[ "Takko", ",", "Aomori", "Prefecture" ]</t>
+  </si>
+  <si>
+    <t>[ 3, 0, 5, 6 ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Takko", "LOC: Aomori Prefecture" ]</t>
+  </si>
+  <si>
+    <t>[ "Stadion", "v", "Jiráskově", "ulici", ",", "Jihlava" ]</t>
+  </si>
+  <si>
+    <t>[ 3, 4, 4, 4, 0, 5 ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Stadion v Jiráskově ulici", "LOC: Jihlava" ]</t>
+  </si>
+  <si>
+    <t>[ "Wayne", "Dowdy", "(", "D", ")" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Wayne Dowdy" ]</t>
+  </si>
+  <si>
+    <t>[ "He", "was", "born", "in", "Bobai", "County", ",", "Guangxi", "." ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 0, 0, 5, 6, 0, 5, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Bobai County", "LOC: Guangxi" ]</t>
+  </si>
+  <si>
+    <t>[ "South", "Windsor", ",", "Connecticut" ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: South Windsor , Connecticut" ]</t>
+  </si>
+  <si>
+    <t>[ "Communes", "of", "the", "Côte-d'Or", "department" ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Communes of the Côte-d'Or department" ]</t>
+  </si>
+  <si>
+    <t>[ "Njenga", "Karume", "(", "2006", "?", "-2008", ")" ]</t>
+  </si>
+  <si>
+    <t>[ 1, 2, 0, 0, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Njenga Karume" ]</t>
+  </si>
+  <si>
+    <t>[ "''", "Holy", "Roman", "Empire", "''", "'", "–", "Leopold", "I", "(", "1658–1705", ")" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 3, 4, 4, 0, 0, 0, 1, 2, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Holy Roman Empire", "PER: Leopold I" ]</t>
+  </si>
+  <si>
+    <t>[ "The", "text", "was", "first", "edited", "by", "Gershom", "Scholem", "(", "1965", ")", "." ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 0, 0, 0, 0, 1, 2, 0, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Gershom Scholem" ]</t>
+  </si>
+  <si>
+    <t>[ "Gregoria", "de", "Jesús", "(", "1978", ")" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Gregoria de Jesús" ]</t>
+  </si>
+  <si>
+    <t>[ "It", "flows", "from", "Ägerisee", "through", "Lake", "Zug", "into", "the", "Reuss", "." ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 0, 5, 0, 5, 6, 0, 0, 5, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Ägerisee", "LOC: Lake Zug", "LOC: Reuss" ]</t>
+  </si>
+  <si>
+    <t>[ "Epoch", "of", "Unlight" ]</t>
+  </si>
+  <si>
+    <t>[ 3, 4, 4 ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Epoch of Unlight" ]</t>
+  </si>
+  <si>
+    <t>[ "Rick", "Rubin", "-", "producer" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Rick Rubin" ]</t>
+  </si>
+  <si>
+    <t>[ "*August", "15", "–", "Mary", "Lou", "Graham" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 0, 1, 2, 2 ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Mary Lou Graham" ]</t>
+  </si>
+  <si>
+    <t>[ "Joseph", "Benavidez", ",", "Head", "Coach" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Joseph Benavidez" ]</t>
+  </si>
+  <si>
+    <t>[ "*Ambassador", "to", "Egypt", ",", "Sudan", "and", "the", "Arab", "League", ":", "1963–1970" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 5, 0, 5, 0, 0, 3, 4, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: Egypt", "LOC: Sudan", "ORG: Arab League" ]</t>
+  </si>
+  <si>
+    <t>[ "***", "Odo", ",", "Count", "of", "Toulouse" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 1, 2, 2, 2, 2 ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Odo , Count of Toulouse" ]</t>
+  </si>
+  <si>
+    <t>[ "**", "Sancho", "II", "(", "1223–1247", ")" ]</t>
+  </si>
+  <si>
+    <t>[ 0, 1, 2, 0, 0, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Sancho II" ]</t>
+  </si>
+  <si>
+    <t>[ "Wesley", "Pruden", "(", "2013", ")" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Wesley Pruden" ]</t>
+  </si>
+  <si>
+    <t>[ "Previews", "are", "scheduled", "to", "begin", "March", "13", ",", "2017", ",", "with", "an", "opening", "date", "of", "April", "20", ",", "2017", ",", "at", "the", "Shubert", "Theatre", "." ]</t>
+  </si>
+  <si>
+    <t>[ 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 3, 4, 0 ]</t>
+  </si>
+  <si>
+    <t>[ "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en", "en" ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Shubert Theatre" ]</t>
+  </si>
+  <si>
+    <t>[ "China", ",", "Indonesia", ",", "Vietnam" ]</t>
+  </si>
+  <si>
+    <t>[ 5, 0, 5, 0, 5 ]</t>
+  </si>
+  <si>
+    <t>[ "LOC: China", "LOC: Indonesia", "LOC: Vietnam" ]</t>
+  </si>
+  <si>
+    <t>[ "Emmett", "/", "Furla", "/", "Oasis", "Films" ]</t>
+  </si>
+  <si>
+    <t>[ "ORG: Emmett / Furla / Oasis Films" ]</t>
+  </si>
+  <si>
+    <t>[ "Ekaterina", "Petaikina", "/", "Maxim", "Kurdyukov" ]</t>
+  </si>
+  <si>
+    <t>[ "PER: Ekaterina Petaikina", "PER: Maxim Kurdyukov" ]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -636,18 +1494,25 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow (Body)"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -662,11 +1527,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,6 +1548,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1001,10 +1871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8794710-C8CC-B840-A1E7-BD3C0386E1F1}">
-  <dimension ref="A1:B127"/>
+  <dimension ref="A1:E202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1013,967 +1883,2623 @@
     <col min="2" max="2" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>142</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>143</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>144</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>145</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>146</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>147</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>148</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>149</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>150</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>151</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>152</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>153</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>154</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>155</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>156</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>157</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>158</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>159</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>160</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>161</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>162</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>165</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>166</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>167</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>170</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>171</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>172</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>173</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>174</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>175</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>176</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>177</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>178</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>180</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>181</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>182</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>183</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>184</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>185</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>186</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>187</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
         <v>182</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>123</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="3" t="s">
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
         <v>188</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>130</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>133</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>134</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>136</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>134</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>134</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>138</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>139</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
         <v>189</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>190</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>141</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B103" s="1"/>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B104" s="1"/>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B105" s="1"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B106" s="1"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B107" s="1"/>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B108" s="1"/>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B109" s="1"/>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B110" s="1"/>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B111" s="1"/>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B112" s="1"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B113" s="1"/>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B114" s="1"/>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B115" s="1"/>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B116" s="1"/>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B117" s="1"/>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B118" s="1"/>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B119" s="1"/>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B120" s="1"/>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B121" s="1"/>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B122" s="1"/>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A123" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B123" s="1"/>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B124" s="1"/>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B125" s="1"/>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B126" s="1"/>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B127" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" s="3"/>
+      <c r="B103" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" s="3"/>
+      <c r="B104" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" s="3"/>
+      <c r="B105" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" s="3"/>
+      <c r="B106" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="3"/>
+      <c r="B107" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" s="3"/>
+      <c r="B108" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" s="3"/>
+      <c r="B109" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" s="3"/>
+      <c r="B110" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" s="3"/>
+      <c r="B111" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" s="3"/>
+      <c r="B112" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" s="3"/>
+      <c r="B113" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" s="3"/>
+      <c r="B114" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" s="3"/>
+      <c r="B115" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" s="3"/>
+      <c r="B116" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117" s="3"/>
+      <c r="B117" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118" s="3"/>
+      <c r="B118" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119" s="3"/>
+      <c r="B119" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" s="3"/>
+      <c r="B120" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" s="3"/>
+      <c r="B121" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122" s="3"/>
+      <c r="B122" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123" s="3"/>
+      <c r="B123" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" s="3"/>
+      <c r="B124" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125" s="3"/>
+      <c r="B125" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126" s="3"/>
+      <c r="B126" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127" s="3"/>
+      <c r="B127" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128" s="3"/>
+      <c r="B128" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129" s="3"/>
+      <c r="B129" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130" s="3"/>
+      <c r="B130" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131" s="3"/>
+      <c r="B131" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132" s="3"/>
+      <c r="B132" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133" s="3"/>
+      <c r="B133" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134" s="3"/>
+      <c r="B134" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135" s="3"/>
+      <c r="B135" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136" s="3"/>
+      <c r="B136" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137" s="3"/>
+      <c r="B137" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138" s="3"/>
+      <c r="B138" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139" s="3"/>
+      <c r="B139" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140" s="3"/>
+      <c r="B140" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141" s="3"/>
+      <c r="B141" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142" s="3"/>
+      <c r="B142" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143" s="3"/>
+      <c r="B143" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144" s="3"/>
+      <c r="B144" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145" s="3"/>
+      <c r="B145" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146" s="3"/>
+      <c r="B146" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147" s="3"/>
+      <c r="B147" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148" s="3"/>
+      <c r="B148" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149" s="3"/>
+      <c r="B149" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150" s="3"/>
+      <c r="B150" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151" s="3"/>
+      <c r="B151" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152" s="3"/>
+      <c r="B152" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153" s="4"/>
+      <c r="B153" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154" s="4"/>
+      <c r="B154" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" s="4"/>
+      <c r="B155" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156" s="4"/>
+      <c r="B156" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157" s="4"/>
+      <c r="B157" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158" s="4"/>
+      <c r="B158" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159" s="4"/>
+      <c r="B159" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160" s="4"/>
+      <c r="B160" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161" s="4"/>
+      <c r="B161" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162" s="4"/>
+      <c r="B162" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163" s="4"/>
+      <c r="B163" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164" s="4"/>
+      <c r="B164" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165" s="4"/>
+      <c r="B165" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166" s="4"/>
+      <c r="B166" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167" s="4"/>
+      <c r="B167" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168" s="4"/>
+      <c r="B168" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A169" s="4"/>
+      <c r="B169" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170" s="4"/>
+      <c r="B170" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171" s="4"/>
+      <c r="B171" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A172" s="4"/>
+      <c r="B172" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173" s="4"/>
+      <c r="B173" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A174" s="4"/>
+      <c r="B174" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A175" s="4"/>
+      <c r="B175" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A176" s="4"/>
+      <c r="B176" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A177" s="4"/>
+      <c r="B177" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A178" s="4"/>
+      <c r="B178" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A179" s="4"/>
+      <c r="B179" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A180" s="4"/>
+      <c r="B180" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A181" s="4"/>
+      <c r="B181" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A182" s="4"/>
+      <c r="B182" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A183" s="4"/>
+      <c r="B183" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A184" s="4"/>
+      <c r="B184" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A185" s="4"/>
+      <c r="B185" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A186" s="4"/>
+      <c r="B186" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A187" s="4"/>
+      <c r="B187" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A188" s="4"/>
+      <c r="B188" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A189" s="4"/>
+      <c r="B189" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A190" s="4"/>
+      <c r="B190" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A191" s="4"/>
+      <c r="B191" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A192" s="4"/>
+      <c r="B192" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A193" s="4"/>
+      <c r="B193" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A194" s="4"/>
+      <c r="B194" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A195" s="4"/>
+      <c r="B195" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A196" s="4"/>
+      <c r="B196" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A197" s="4"/>
+      <c r="B197" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A198" s="4"/>
+      <c r="B198" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A199" s="4"/>
+      <c r="B199" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A200" s="4"/>
+      <c r="B200" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A201" s="4"/>
+      <c r="B201" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A202" s="4"/>
+      <c r="B202" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>476</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>